<commit_message>
Updated data and script files
</commit_message>
<xml_diff>
--- a/Meta-Analysis-PANSS-data.xlsx
+++ b/Meta-Analysis-PANSS-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://syddanskuni-my.sharepoint.com/personal/cstrozza_health_sdu_dk/Documents/_Other projects/PANSS meta analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4DC874B8-D88A-45C8-BD28-F964159B846D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{4DC874B8-D88A-45C8-BD28-F964159B846D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00C3A118-9282-4665-AE5A-59D4B8AAB813}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-135" windowWidth="29040" windowHeight="15840" xr2:uid="{5E15E32C-A49E-4676-9033-2CE1F8795441}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5E15E32C-A49E-4676-9033-2CE1F8795441}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -296,7 +296,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -343,7 +343,9 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{85DE360E-0A4D-4FBB-ADD6-B7BB7BDA45C0}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -655,7 +657,7 @@
   <dimension ref="A1:AJ28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1143,7 +1145,7 @@
         <v>45</v>
       </c>
       <c r="B5">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="C5" t="s">
         <v>44</v>

</xml_diff>